<commit_message>
added css  checker for the sidebar icons
</commit_message>
<xml_diff>
--- a/Excel/Productnumbers.xlsx
+++ b/Excel/Productnumbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rothm/Desktop/PP_Automated_Tests/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF3F27E-B666-AE49-B8D8-314E06F1C09D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D3C794-B658-934F-892D-A7AFA68544F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" firstSheet="6" activeTab="6" xr2:uid="{A98BA704-44FB-7246-8FB0-5F450B575435}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" activeTab="2" xr2:uid="{A98BA704-44FB-7246-8FB0-5F450B575435}"/>
   </bookViews>
   <sheets>
     <sheet name="redPriceTag" sheetId="1" r:id="rId1"/>
@@ -34,6 +34,7 @@
     <sheet name="set" sheetId="18" r:id="rId19"/>
     <sheet name="new" sheetId="19" r:id="rId20"/>
     <sheet name="ProductName" sheetId="20" r:id="rId21"/>
+    <sheet name="Sheet1" sheetId="22" r:id="rId22"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -1560,12 +1561,24 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DE8CA9-DC83-A943-8B6C-32190BCAE540}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47D19AC8-8CD9-DD4C-93EF-B8B9DB71C8A5}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="A7:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1635,10 +1648,6 @@
       <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1883,8 +1892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6598092F-A871-8A40-9119-0E94E0F3E9D3}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>